<commit_message>
Code Cleanup, Accelerometer Documentation, Cost and Collab Updates
</commit_message>
<xml_diff>
--- a/Documents/Report Material/Collaboration and Hours.xlsx
+++ b/Documents/Report Material/Collaboration and Hours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aj39a\Documents\GitHub\ECE-371-Project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aj39a\Documents\GitHub\ECE-371-Project\Documents\Report Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6946E2A-8473-42C4-96DC-26D23FF1B9EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDE43CD-87B0-4646-8C14-8E8F0793A843}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="2370" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33030" yWindow="1440" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Block</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>N/C</t>
   </si>
   <si>
     <t>Speaker Driver</t>
@@ -407,7 +404,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,39 +453,48 @@
       <c r="D2" s="1">
         <v>43795</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
+      <c r="E2" s="1">
+        <v>43802</v>
       </c>
       <c r="F2">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
       <c r="D3" s="1">
         <v>43795</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43794</v>
+      </c>
+      <c r="F3">
+        <v>35</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <v>43795</v>
@@ -505,10 +511,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -528,10 +534,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>

</xml_diff>